<commit_message>
plotting graph a create dicts for printing erg
</commit_message>
<xml_diff>
--- a/hhdaten/bewegungsdaten.xlsx
+++ b/hhdaten/bewegungsdaten.xlsx
@@ -12,6 +12,9 @@
     <sheet name="Produkt" sheetId="2" r:id="rId3"/>
     <sheet name="erl" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planung!$A$1:$S$1116</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -6695,7 +6698,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -6705,8 +6708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S1116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -72556,6 +72559,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:S1116"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -78046,7 +78050,7 @@
   <dimension ref="A1:I314"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="A1:H23"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>